<commit_message>
add new img v6
</commit_message>
<xml_diff>
--- a/ID_SanPham._ChanGa.xlsx
+++ b/ID_SanPham._ChanGa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ChanGa_Personal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0128B2-82D9-4EFB-99BC-E35F74E9260B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5652455-CCEF-4F6D-BFD6-F469E176BD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D6F5E742-A921-4C78-A2CA-E7DD1F27105C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="799">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="807">
   <si>
     <t>ID</t>
   </si>
@@ -3380,9 +3380,6 @@
     <t>for /l %i in (1,1,16) do mkdir  %folder%_%i</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>𝗟𝗢𝗩𝗘 𝗔𝗡𝗗 𝗠𝗘
 ✈︎ Đặt ngay một vé hạng thương gia bay thẳng đến trái tim nàng với set chăn ga gối Lụa thượng hạng Love and Me mới nhất! 
 🌹 Như minh chứng cho tình yêu, set chăn ga có hoạ tiết vân chìm và đường thêu logo nổi  tuyệt đẹp, chất liệu vải sợi 100s vô cùng bền bỉ nhưng lại rất mềm và mịn
@@ -3512,6 +3509,62 @@
 • 1 ga tấm trải giường free size
 • 1 vỏ chăn 200x230cm (khóa kéo)
 • 2 vỏ gối đầu 50x70cm</t>
+  </si>
+  <si>
+    <t>🌙 Cologne | Midnight in Paris – Paris về đêm| Hàng ga chần sẵn
+🎞️ Tựa như một khung hình trong phim cổ điển Pháp
+💋 Gam hồng trầm quyến rũ kết hợp hoa văn cổ điển Á – Âu như những thước phim từ thập niên vàng son. Từng cánh hoa như khắc họa câu chuyện tình ẩn giấu trong ánh đèn vàng mờ ảo của Paris lúc nửa đêm.
+✨ Chi tiết chất liệu cao cấp:
+Mặt A: 🫧 Lụa satin tự nhiên – mềm mịn, mượt mà
+Mặt B: 🍃 Tencel cotton – mát lành, thoáng khí
+Kỹ thuật: 🎨 In kỹ thuật số + YKK khóa kéo</t>
+  </si>
+  <si>
+    <t>Sỉ sẵn sll 530 540 560</t>
+  </si>
+  <si>
+    <t>Hot new 2025❄️❄️
+Dòng vải thế hệ mới lần đầu tiên xuất hiện ✨👌
+Cotton linen 3 chiều Magnetic mặt vải sợi lanh đc dệt từ cây gai dầu đanh mịn mềm mát chống ẩm mốc cực kì hiệu quả kết hợp phong cách trần bông hàn quốc sang trọng 🇰🇷
+Đặc biệt chăn chần vẫn có khoá kéo lồng dc ruột cực kì tiện lợi
+Thật sự rất xứng đáng để trải nghiệm 🫧
+Full set 5 món 
+-1 chăn trần 200*230cm có khoá kéo lồng ruột
+-2 vỏ gối trần 48*74cm
+-1 ga chun trần ( m6 -m8 -2m2 cao 25cm )
+1 vỏ ôm trần bông 48*74cm</t>
+  </si>
+  <si>
+    <t>ập nhật  ga gối cotton living về bù 16 mau fullsize 
+Cotton living thì vải quá nhiều ưu điểm ko cần giới thiệu nhiều ạ ;p ;p 
+cứ cotton dùng yên tâm tuyệt đối 💯</t>
+  </si>
+  <si>
+    <t>for /f %%I in ("%cd%") do set folder=%%~nxI</t>
+  </si>
+  <si>
+    <t>for /l %%i in (1,1,%1) do mkdir  %folder%_%%i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">call  F:\make_folder.bat </t>
+  </si>
+  <si>
+    <t>✨ MỘNG YÊN NHIÊN - TENCEL THÊU CAO CẤP ✨
+BST Xuân Hè mới – Lấy cảm hứng từ khăn lụa hoa thương hiệu H
+🌸 Thêu hoa nghệ thuật - Nữ tính đầy tinh tế
+Mẫu hoa thêu tỉ mỉ trên nền Tencel mềm mượt, sang trọng, từng đường kim như bước ra từ thời trang cao cấp.
+Tone xanh non nhẹ nhàng – hợp từ phòng đơn giản đến hiện đại.
+☁️ Chất liệu 100% Tencel Lenzing – mát lạnh như lụa thật
+ • Mỏng nhẹ chỉ 0.1mm
+ • Thoáng khí, khô ráo
+ • Dịu mát suốt đêm hè
+Set gồm:
+ • 1 vỏ chăn 200x230 (thêu cao cấp)
+ • 1 ga trải giường 245x250
+ • 2 vỏ gối đầu 50x70</t>
+  </si>
+  <si>
+    <t>730 750 780</t>
   </si>
 </sst>
 </file>
@@ -4297,8 +4350,8 @@
   <dimension ref="A1:J270"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K197" sqref="K197"/>
+      <pane ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C225" sqref="C225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4978,7 +5031,7 @@
         <v>𝐍ế𝐮 𝐞𝐦 𝐭𝐡𝐢́𝐜𝐡 𝐬ự 𝐥𝐚̃𝐧𝐠 𝐦ạ𝐧 𝐜ủ𝐚 𝐂𝐡𝐚̂𝐮 𝐀̂𝐮 𝐡𝐚̃𝐲 đế𝐧 đ𝐚̂𝐲 𝐯ớ𝐢 𝐚𝐧𝐡✨</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A79" s="33" t="s">
         <v>13</v>
       </c>
@@ -5602,7 +5655,7 @@
         <v>✨ CHĂN GA LỤA THÊU BÁNH BÈO – NÀNG CÔNG CHÚA TRONG MƠ ✨</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>50</v>
       </c>
@@ -5992,7 +6045,7 @@
 Đáng yêu như Min Min - Thắp ánh đèn bật tình yêu lên </v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>74</v>
       </c>
@@ -6137,7 +6190,7 @@
         <v>Họa Tiết Nghệ Thuật Huyền Diệu</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>82</v>
       </c>
@@ -6257,7 +6310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>89</v>
       </c>
@@ -6799,7 +6852,7 @@
         <v>TENCEL MARK CROSS 100S ĐÍNH ĐÁ Ga trần nhập khẩu- KHẲNG ĐỊNH PHONG CÁCH, NÂNG TẦM KHÔNG GIAN</v>
       </c>
     </row>
-    <row r="186" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>448</v>
       </c>
@@ -6839,7 +6892,7 @@
       </c>
       <c r="B188" s="1"/>
       <c r="C188" s="4" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="D188" s="1">
         <v>2100</v>
@@ -6855,7 +6908,7 @@
       </c>
       <c r="B189" s="1"/>
       <c r="C189" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D189" s="1">
         <v>1650</v>
@@ -6870,10 +6923,10 @@
         <v>452</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D190" s="1">
         <v>2450</v>
@@ -6888,13 +6941,13 @@
         <v>453</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C191" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D191" s="1" t="s">
         <v>789</v>
-      </c>
-      <c r="D191" s="1" t="s">
-        <v>790</v>
       </c>
       <c r="E191" s="38" t="str">
         <f t="shared" si="4"/>
@@ -6906,10 +6959,10 @@
         <v>454</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="D192" s="1">
         <v>1950</v>
@@ -6942,7 +6995,7 @@
       </c>
       <c r="B194" s="1"/>
       <c r="C194" s="4" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D194" s="1">
         <v>1950</v>
@@ -6958,7 +7011,7 @@
       </c>
       <c r="B195" s="1"/>
       <c r="C195" s="4" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D195" s="1">
         <v>2000</v>
@@ -6974,7 +7027,7 @@
       </c>
       <c r="B196" s="1"/>
       <c r="C196" s="4" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="D196" s="1">
         <v>2650</v>
@@ -6990,7 +7043,7 @@
       </c>
       <c r="B197" s="1"/>
       <c r="C197" s="4" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D197" s="1">
         <v>1950</v>
@@ -7006,7 +7059,7 @@
       </c>
       <c r="B198" s="1"/>
       <c r="C198" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D198" s="1">
         <v>1700</v>
@@ -7016,49 +7069,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>461</v>
       </c>
       <c r="B199" s="1"/>
-      <c r="C199" s="4"/>
-      <c r="D199" s="1"/>
+      <c r="C199" s="4" t="s">
+        <v>798</v>
+      </c>
+      <c r="D199" s="1">
+        <v>2300</v>
+      </c>
       <c r="E199" s="38">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>462</v>
       </c>
       <c r="B200" s="1"/>
-      <c r="C200" s="4"/>
-      <c r="D200" s="1"/>
+      <c r="C200" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>799</v>
+      </c>
       <c r="E200" s="38">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>463</v>
       </c>
       <c r="B201" s="1"/>
-      <c r="C201" s="4"/>
-      <c r="D201" s="1"/>
+      <c r="C201" s="4" t="s">
+        <v>800</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>806</v>
+      </c>
       <c r="E201" s="38">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" ht="240" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>464</v>
       </c>
       <c r="B202" s="1"/>
-      <c r="C202" s="4"/>
-      <c r="D202" s="1"/>
+      <c r="C202" s="4" t="s">
+        <v>805</v>
+      </c>
+      <c r="D202" s="1">
+        <v>2000</v>
+      </c>
       <c r="E202" s="38">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -7069,9 +7138,7 @@
         <v>465</v>
       </c>
       <c r="B203" s="1"/>
-      <c r="C203" s="4" t="s">
-        <v>784</v>
-      </c>
+      <c r="C203" s="4"/>
       <c r="D203" s="1"/>
       <c r="E203" s="38">
         <f t="shared" si="4"/>
@@ -7938,30 +8005,42 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C48B2C-3B71-4A97-889A-14151471C093}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>782</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>783</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>804</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new img hihi
</commit_message>
<xml_diff>
--- a/ID_SanPham._ChanGa.xlsx
+++ b/ID_SanPham._ChanGa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ChanGa_Personal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3459B1-771B-43AA-9EF9-D46B7F3DC3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA60899-A0CC-4A0F-9698-085321959281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D6F5E742-A921-4C78-A2CA-E7DD1F27105C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="812">
   <si>
     <t>ID</t>
   </si>
@@ -3591,6 +3591,44 @@
  • 01 chăn hè thêu 200×230
  • 02 vỏ gối 50×70
  • 01 ga trải giường free size</t>
+  </si>
+  <si>
+    <t>🌸 Bộ sưu tập 2025
+NO.15 – Helena Light Pink
+Set 4 món
+-1 chăn hè tơ tằm
+-1 ga chần sẵn
+-2 vỏ gối nằm
+“Chạm khẽ sắc xuân, đánh thức vẻ đẹp ẩn sâu trong sự tối giản.”
+Một thiết kế hiện đại kết hợp tinh thần lãng mạn mùa xuân mang đến trải nghiệm nghỉ ngơi đầy cảm xúc. Vải mềm mượt, nhẹ tênh như tơ trời, điểm xuyết chi tiết thêu tinh tế mà không rườm rà.
+✨ Chất liệu vượt trội:
+ • Vải: 65% Tencel Lenzing + 35% Cotton
+ • Ruột chăn: 15% Silk(tơ tằm) tự nhiên + 85% sợi polyester siêu nhẹ
+ • Công nghệ: Laser cắt hoa Italy + thêu không giấy cao cấp
+Tone màu nhẹ nhàng:
+🎀 Hồng phấn nhẹ – Tươi mới, đầy nữ tính
+🌫 Xám khói – Lịch lãm và hiện đại
+🕊 Trắng tinh khôi – Tối giản chuẩn châu Âu
+🍃 Xanh mint – Tươi mát, thanh thoát
+☁️ Kem sữa – Nhẹ nhàng như sương mai
+🌷 Tím pastel – Dịu dàng, đầy chất thơ
+💬 “Less is more” – khi bạn chọn sự đơn giản, bạn đang chọn đẳng cấp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">𝗠𝗔𝗥𝗞 𝗖𝗥𝗢𝗦𝗦Maloch·𝐍𝐄𝐖Sản phẩm mới mùa xuân hè · đơn giản thêu nhẹ nhàng sang trọng #[Agnes] tinh tế 𝐍𝐎.seri 6
+[Agne]
+Telcel lụa 80s Detail🌿
+Cảm hứng thiết kế:
+Hình thêu trang nhã trên cành và lá tạo nên phong cách duyên dáng sử dụng hình dạng cây nho để thể hiện vẻ đẹp sang trong và hơi thở sống động của thời đại.🔔🔔
+♣️màu sắc trang nhã, đường thêu tỉ mỉ, tô điểm bằng chỉ thêu ánh kim toát kết hợp những đường thêu tinh tế 🔝🔝
+Set 4 món full 3 màu
+-1 ga freesize 245*250cm
+-1 vỏ chăn 200*230cm
+-2 vỏ gối nằm 48*74
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cotton fabric mới đẹp</t>
   </si>
 </sst>
 </file>
@@ -3986,40 +4024,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4057,6 +4062,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4376,8 +4414,8 @@
   <dimension ref="A1:J270"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D204" sqref="D204"/>
+      <pane ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D208" sqref="D208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4414,19 +4452,19 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="56" t="s">
         <v>180</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="D2" s="61">
+      <c r="D2" s="50">
         <v>1700</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="47" t="s">
         <v>186</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -4434,610 +4472,610 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="65"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="59"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="48"/>
       <c r="J3" s="2" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="65"/>
-      <c r="B4" s="68"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="59"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="48"/>
       <c r="J4" s="2" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="65"/>
-      <c r="B5" s="68"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="59"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="48"/>
       <c r="J5" s="2" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="65"/>
-      <c r="B6" s="68"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="59"/>
+      <c r="A6" s="54"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="48"/>
       <c r="J6" s="2" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="65"/>
-      <c r="B7" s="68"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="59"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="48"/>
       <c r="J7" s="2" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="65"/>
-      <c r="B8" s="68"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="59"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="48"/>
       <c r="J8" s="2" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="65"/>
-      <c r="B9" s="68"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="59"/>
+      <c r="A9" s="54"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="48"/>
       <c r="J9" s="2" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="65"/>
-      <c r="B10" s="68"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="59"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="48"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="66"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="60"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="49"/>
     </row>
     <row r="12" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="D12" s="47">
+      <c r="D12" s="60">
         <v>1950</v>
       </c>
-      <c r="E12" s="49" t="s">
+      <c r="E12" s="59" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="54"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="49"/>
+      <c r="A13" s="62"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="59"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="49"/>
+      <c r="A14" s="62"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="59"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="54"/>
-      <c r="B15" s="47"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="49"/>
+      <c r="A15" s="62"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="59"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
-      <c r="B16" s="47"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="49"/>
+      <c r="A16" s="62"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="59"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="49"/>
+      <c r="A17" s="62"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="59"/>
     </row>
     <row r="18" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="54"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="49"/>
+      <c r="A18" s="62"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="59"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="54"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="49"/>
+      <c r="A19" s="62"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="59"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="54"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="49"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="59"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="54"/>
-      <c r="B21" s="47"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="49"/>
+      <c r="A21" s="62"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="59"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="54"/>
-      <c r="B22" s="47"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="49"/>
+      <c r="A22" s="62"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="59"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="54"/>
-      <c r="B23" s="47"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="49"/>
+      <c r="A23" s="62"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="59"/>
     </row>
     <row r="24" spans="1:5" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="60" t="s">
         <v>184</v>
       </c>
-      <c r="C24" s="55" t="s">
+      <c r="C24" s="64" t="s">
         <v>228</v>
       </c>
-      <c r="D24" s="48">
+      <c r="D24" s="63">
         <v>2300</v>
       </c>
-      <c r="E24" s="49" t="s">
+      <c r="E24" s="59" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="46"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="49"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="59"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="46"/>
-      <c r="B26" s="47"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="49"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="59"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="46"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="49"/>
+      <c r="A27" s="61"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="59"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="46"/>
-      <c r="B28" s="47"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="49"/>
+      <c r="A28" s="61"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="59"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="46"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="49"/>
+      <c r="A29" s="61"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="59"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="46"/>
-      <c r="B30" s="47"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="49"/>
+      <c r="A30" s="61"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="59"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="46"/>
-      <c r="B31" s="47"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="49"/>
+      <c r="A31" s="61"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="59"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="46"/>
-      <c r="B32" s="47"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="49"/>
+      <c r="A32" s="61"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="59"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="46"/>
-      <c r="B33" s="47"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="49"/>
+      <c r="A33" s="61"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="59"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="46"/>
-      <c r="B34" s="47"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="49"/>
+      <c r="A34" s="61"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="59"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="46"/>
-      <c r="B35" s="47"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="49"/>
+      <c r="A35" s="61"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="59"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="46" t="s">
+      <c r="A36" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="60" t="s">
         <v>185</v>
       </c>
-      <c r="C36" s="50" t="s">
+      <c r="C36" s="67" t="s">
         <v>229</v>
       </c>
-      <c r="D36" s="47">
+      <c r="D36" s="60">
         <v>1700</v>
       </c>
-      <c r="E36" s="49" t="s">
+      <c r="E36" s="59" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="46"/>
-      <c r="B37" s="47"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="49"/>
+      <c r="A37" s="61"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="68"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="59"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="46"/>
-      <c r="B38" s="47"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="49"/>
+      <c r="A38" s="61"/>
+      <c r="B38" s="60"/>
+      <c r="C38" s="68"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="59"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="46"/>
-      <c r="B39" s="47"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="49"/>
+      <c r="A39" s="61"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="60"/>
+      <c r="E39" s="59"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="46"/>
-      <c r="B40" s="47"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="49"/>
+      <c r="A40" s="61"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="59"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="46"/>
-      <c r="B41" s="47"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="49"/>
+      <c r="A41" s="61"/>
+      <c r="B41" s="60"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="59"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="46"/>
-      <c r="B42" s="47"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="49"/>
+      <c r="A42" s="61"/>
+      <c r="B42" s="60"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="59"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="46"/>
-      <c r="B43" s="47"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="47"/>
-      <c r="E43" s="49"/>
+      <c r="A43" s="61"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="59"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="46"/>
-      <c r="B44" s="47"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="47"/>
-      <c r="E44" s="49"/>
+      <c r="A44" s="61"/>
+      <c r="B44" s="60"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="60"/>
+      <c r="E44" s="59"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="46"/>
-      <c r="B45" s="47"/>
-      <c r="C45" s="52"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="49"/>
+      <c r="A45" s="61"/>
+      <c r="B45" s="60"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="59"/>
     </row>
     <row r="46" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="46" t="s">
+      <c r="A46" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="B46" s="47" t="s">
+      <c r="B46" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="C46" s="50" t="s">
+      <c r="C46" s="67" t="s">
         <v>230</v>
       </c>
-      <c r="D46" s="47">
+      <c r="D46" s="60">
         <v>1950</v>
       </c>
-      <c r="E46" s="49" t="s">
+      <c r="E46" s="59" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="46"/>
-      <c r="B47" s="47"/>
-      <c r="C47" s="51"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="49"/>
+      <c r="A47" s="61"/>
+      <c r="B47" s="60"/>
+      <c r="C47" s="68"/>
+      <c r="D47" s="60"/>
+      <c r="E47" s="59"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="46"/>
-      <c r="B48" s="47"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="47"/>
-      <c r="E48" s="49"/>
+      <c r="A48" s="61"/>
+      <c r="B48" s="60"/>
+      <c r="C48" s="68"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="59"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="46"/>
-      <c r="B49" s="47"/>
-      <c r="C49" s="51"/>
-      <c r="D49" s="47"/>
-      <c r="E49" s="49"/>
+      <c r="A49" s="61"/>
+      <c r="B49" s="60"/>
+      <c r="C49" s="68"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="59"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="46"/>
-      <c r="B50" s="47"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="47"/>
-      <c r="E50" s="49"/>
+      <c r="A50" s="61"/>
+      <c r="B50" s="60"/>
+      <c r="C50" s="68"/>
+      <c r="D50" s="60"/>
+      <c r="E50" s="59"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="46"/>
-      <c r="B51" s="47"/>
-      <c r="C51" s="51"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="49"/>
+      <c r="A51" s="61"/>
+      <c r="B51" s="60"/>
+      <c r="C51" s="68"/>
+      <c r="D51" s="60"/>
+      <c r="E51" s="59"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="46"/>
-      <c r="B52" s="47"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="47"/>
-      <c r="E52" s="49"/>
+      <c r="A52" s="61"/>
+      <c r="B52" s="60"/>
+      <c r="C52" s="68"/>
+      <c r="D52" s="60"/>
+      <c r="E52" s="59"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="46"/>
-      <c r="B53" s="47"/>
-      <c r="C53" s="51"/>
-      <c r="D53" s="47"/>
-      <c r="E53" s="49"/>
+      <c r="A53" s="61"/>
+      <c r="B53" s="60"/>
+      <c r="C53" s="68"/>
+      <c r="D53" s="60"/>
+      <c r="E53" s="59"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="46"/>
-      <c r="B54" s="47"/>
-      <c r="C54" s="52"/>
-      <c r="D54" s="47"/>
-      <c r="E54" s="49"/>
+      <c r="A54" s="61"/>
+      <c r="B54" s="60"/>
+      <c r="C54" s="69"/>
+      <c r="D54" s="60"/>
+      <c r="E54" s="59"/>
     </row>
     <row r="55" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="46" t="s">
+      <c r="A55" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="B55" s="47" t="s">
+      <c r="B55" s="60" t="s">
         <v>189</v>
       </c>
-      <c r="C55" s="50" t="s">
+      <c r="C55" s="67" t="s">
         <v>231</v>
       </c>
-      <c r="D55" s="47">
+      <c r="D55" s="60">
         <v>1650</v>
       </c>
-      <c r="E55" s="49" t="s">
+      <c r="E55" s="59" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="46"/>
-      <c r="B56" s="47"/>
-      <c r="C56" s="51"/>
-      <c r="D56" s="47"/>
-      <c r="E56" s="49"/>
+      <c r="A56" s="61"/>
+      <c r="B56" s="60"/>
+      <c r="C56" s="68"/>
+      <c r="D56" s="60"/>
+      <c r="E56" s="59"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="46"/>
-      <c r="B57" s="47"/>
-      <c r="C57" s="51"/>
-      <c r="D57" s="47"/>
-      <c r="E57" s="49"/>
+      <c r="A57" s="61"/>
+      <c r="B57" s="60"/>
+      <c r="C57" s="68"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="59"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="46"/>
-      <c r="B58" s="47"/>
-      <c r="C58" s="51"/>
-      <c r="D58" s="47"/>
-      <c r="E58" s="49"/>
+      <c r="A58" s="61"/>
+      <c r="B58" s="60"/>
+      <c r="C58" s="68"/>
+      <c r="D58" s="60"/>
+      <c r="E58" s="59"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="46"/>
-      <c r="B59" s="47"/>
-      <c r="C59" s="51"/>
-      <c r="D59" s="47"/>
-      <c r="E59" s="49"/>
+      <c r="A59" s="61"/>
+      <c r="B59" s="60"/>
+      <c r="C59" s="68"/>
+      <c r="D59" s="60"/>
+      <c r="E59" s="59"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="46"/>
-      <c r="B60" s="47"/>
-      <c r="C60" s="51"/>
-      <c r="D60" s="47"/>
-      <c r="E60" s="49"/>
+      <c r="A60" s="61"/>
+      <c r="B60" s="60"/>
+      <c r="C60" s="68"/>
+      <c r="D60" s="60"/>
+      <c r="E60" s="59"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="46"/>
-      <c r="B61" s="47"/>
-      <c r="C61" s="51"/>
-      <c r="D61" s="47"/>
-      <c r="E61" s="49"/>
+      <c r="A61" s="61"/>
+      <c r="B61" s="60"/>
+      <c r="C61" s="68"/>
+      <c r="D61" s="60"/>
+      <c r="E61" s="59"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="46"/>
-      <c r="B62" s="47"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="47"/>
-      <c r="E62" s="49"/>
+      <c r="A62" s="61"/>
+      <c r="B62" s="60"/>
+      <c r="C62" s="68"/>
+      <c r="D62" s="60"/>
+      <c r="E62" s="59"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="46"/>
-      <c r="B63" s="47"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="47"/>
-      <c r="E63" s="49"/>
+      <c r="A63" s="61"/>
+      <c r="B63" s="60"/>
+      <c r="C63" s="68"/>
+      <c r="D63" s="60"/>
+      <c r="E63" s="59"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="46"/>
-      <c r="B64" s="47"/>
-      <c r="C64" s="51"/>
-      <c r="D64" s="47"/>
-      <c r="E64" s="49"/>
+      <c r="A64" s="61"/>
+      <c r="B64" s="60"/>
+      <c r="C64" s="68"/>
+      <c r="D64" s="60"/>
+      <c r="E64" s="59"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="46"/>
-      <c r="B65" s="47"/>
-      <c r="C65" s="51"/>
-      <c r="D65" s="47"/>
-      <c r="E65" s="49"/>
+      <c r="A65" s="61"/>
+      <c r="B65" s="60"/>
+      <c r="C65" s="68"/>
+      <c r="D65" s="60"/>
+      <c r="E65" s="59"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="46"/>
-      <c r="B66" s="47"/>
-      <c r="C66" s="51"/>
-      <c r="D66" s="47"/>
-      <c r="E66" s="49"/>
+      <c r="A66" s="61"/>
+      <c r="B66" s="60"/>
+      <c r="C66" s="68"/>
+      <c r="D66" s="60"/>
+      <c r="E66" s="59"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="46"/>
-      <c r="B67" s="47"/>
-      <c r="C67" s="52"/>
-      <c r="D67" s="47"/>
-      <c r="E67" s="49"/>
+      <c r="A67" s="61"/>
+      <c r="B67" s="60"/>
+      <c r="C67" s="69"/>
+      <c r="D67" s="60"/>
+      <c r="E67" s="59"/>
     </row>
     <row r="68" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="46" t="s">
+      <c r="A68" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="B68" s="47" t="s">
+      <c r="B68" s="60" t="s">
         <v>191</v>
       </c>
-      <c r="C68" s="50" t="s">
+      <c r="C68" s="67" t="s">
         <v>232</v>
       </c>
-      <c r="D68" s="48">
+      <c r="D68" s="63">
         <v>1850</v>
       </c>
-      <c r="E68" s="49" t="s">
+      <c r="E68" s="59" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="46"/>
-      <c r="B69" s="47"/>
-      <c r="C69" s="51"/>
-      <c r="D69" s="48"/>
-      <c r="E69" s="49"/>
+      <c r="A69" s="61"/>
+      <c r="B69" s="60"/>
+      <c r="C69" s="68"/>
+      <c r="D69" s="63"/>
+      <c r="E69" s="59"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="46"/>
-      <c r="B70" s="47"/>
-      <c r="C70" s="51"/>
-      <c r="D70" s="48"/>
-      <c r="E70" s="49"/>
+      <c r="A70" s="61"/>
+      <c r="B70" s="60"/>
+      <c r="C70" s="68"/>
+      <c r="D70" s="63"/>
+      <c r="E70" s="59"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="46"/>
-      <c r="B71" s="47"/>
-      <c r="C71" s="51"/>
-      <c r="D71" s="48"/>
-      <c r="E71" s="49"/>
+      <c r="A71" s="61"/>
+      <c r="B71" s="60"/>
+      <c r="C71" s="68"/>
+      <c r="D71" s="63"/>
+      <c r="E71" s="59"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="46"/>
-      <c r="B72" s="47"/>
-      <c r="C72" s="51"/>
-      <c r="D72" s="48"/>
-      <c r="E72" s="49"/>
+      <c r="A72" s="61"/>
+      <c r="B72" s="60"/>
+      <c r="C72" s="68"/>
+      <c r="D72" s="63"/>
+      <c r="E72" s="59"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="46"/>
-      <c r="B73" s="47"/>
-      <c r="C73" s="51"/>
-      <c r="D73" s="48"/>
-      <c r="E73" s="49"/>
+      <c r="A73" s="61"/>
+      <c r="B73" s="60"/>
+      <c r="C73" s="68"/>
+      <c r="D73" s="63"/>
+      <c r="E73" s="59"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="46"/>
-      <c r="B74" s="47"/>
-      <c r="C74" s="51"/>
-      <c r="D74" s="48"/>
-      <c r="E74" s="49"/>
+      <c r="A74" s="61"/>
+      <c r="B74" s="60"/>
+      <c r="C74" s="68"/>
+      <c r="D74" s="63"/>
+      <c r="E74" s="59"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="46"/>
-      <c r="B75" s="47"/>
-      <c r="C75" s="51"/>
-      <c r="D75" s="48"/>
-      <c r="E75" s="49"/>
+      <c r="A75" s="61"/>
+      <c r="B75" s="60"/>
+      <c r="C75" s="68"/>
+      <c r="D75" s="63"/>
+      <c r="E75" s="59"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="46"/>
-      <c r="B76" s="47"/>
-      <c r="C76" s="51"/>
-      <c r="D76" s="48"/>
-      <c r="E76" s="49"/>
+      <c r="A76" s="61"/>
+      <c r="B76" s="60"/>
+      <c r="C76" s="68"/>
+      <c r="D76" s="63"/>
+      <c r="E76" s="59"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="46"/>
-      <c r="B77" s="47"/>
-      <c r="C77" s="52"/>
-      <c r="D77" s="48"/>
-      <c r="E77" s="49"/>
+      <c r="A77" s="61"/>
+      <c r="B77" s="60"/>
+      <c r="C77" s="69"/>
+      <c r="D77" s="63"/>
+      <c r="E77" s="59"/>
     </row>
     <row r="78" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A78" s="33" t="s">
@@ -7191,25 +7229,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" ht="390" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>467</v>
       </c>
       <c r="B205" s="1"/>
-      <c r="C205" s="4"/>
-      <c r="D205" s="1"/>
+      <c r="C205" s="4" t="s">
+        <v>809</v>
+      </c>
+      <c r="D205" s="1">
+        <v>2650</v>
+      </c>
       <c r="E205" s="38">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>468</v>
       </c>
       <c r="B206" s="1"/>
-      <c r="C206" s="4"/>
-      <c r="D206" s="1"/>
+      <c r="C206" s="4" t="s">
+        <v>810</v>
+      </c>
+      <c r="D206" s="1">
+        <v>2300</v>
+      </c>
       <c r="E206" s="38">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -7220,8 +7266,12 @@
         <v>469</v>
       </c>
       <c r="B207" s="1"/>
-      <c r="C207" s="4"/>
-      <c r="D207" s="1"/>
+      <c r="C207" s="4" t="s">
+        <v>811</v>
+      </c>
+      <c r="D207" s="1">
+        <v>580</v>
+      </c>
       <c r="E207" s="38">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -7986,17 +8036,16 @@
   </sheetData>
   <autoFilter ref="D1:D270" xr:uid="{4B77AF4A-863B-4858-8141-65534D476F71}"/>
   <mergeCells count="35">
-    <mergeCell ref="C2:C11"/>
-    <mergeCell ref="E2:E11"/>
-    <mergeCell ref="D2:D11"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="B2:B11"/>
-    <mergeCell ref="E36:E45"/>
-    <mergeCell ref="E46:E54"/>
-    <mergeCell ref="E24:E35"/>
-    <mergeCell ref="E12:E23"/>
-    <mergeCell ref="B36:B45"/>
-    <mergeCell ref="D36:D45"/>
+    <mergeCell ref="A68:A77"/>
+    <mergeCell ref="B68:B77"/>
+    <mergeCell ref="D68:D77"/>
+    <mergeCell ref="E68:E77"/>
+    <mergeCell ref="E55:E67"/>
+    <mergeCell ref="D55:D67"/>
+    <mergeCell ref="B55:B67"/>
+    <mergeCell ref="A55:A67"/>
+    <mergeCell ref="C55:C67"/>
+    <mergeCell ref="C68:C77"/>
     <mergeCell ref="A36:A45"/>
     <mergeCell ref="B46:B54"/>
     <mergeCell ref="D46:D54"/>
@@ -8011,16 +8060,17 @@
     <mergeCell ref="C24:C35"/>
     <mergeCell ref="C36:C45"/>
     <mergeCell ref="C46:C54"/>
-    <mergeCell ref="A68:A77"/>
-    <mergeCell ref="B68:B77"/>
-    <mergeCell ref="D68:D77"/>
-    <mergeCell ref="E68:E77"/>
-    <mergeCell ref="E55:E67"/>
-    <mergeCell ref="D55:D67"/>
-    <mergeCell ref="B55:B67"/>
-    <mergeCell ref="A55:A67"/>
-    <mergeCell ref="C55:C67"/>
-    <mergeCell ref="C68:C77"/>
+    <mergeCell ref="E36:E45"/>
+    <mergeCell ref="E46:E54"/>
+    <mergeCell ref="E24:E35"/>
+    <mergeCell ref="E12:E23"/>
+    <mergeCell ref="B36:B45"/>
+    <mergeCell ref="D36:D45"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="E2:E11"/>
+    <mergeCell ref="D2:D11"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="B2:B11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>